<commit_message>
setting up landing, register and login pages
</commit_message>
<xml_diff>
--- a/major_milestones.xlsx
+++ b/major_milestones.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9d1f815b88be513d/Documents/Goldsmiths^J University of London/Year 4/Final Project in Computing (IS53062A)/cultural_manners_mentor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="8_{FE9455B0-5B2A-4DB4-82A5-15E64594C531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62F4FF35-A1FC-498C-8287-7A468A98F4C7}"/>
+  <xr:revisionPtr revIDLastSave="164" documentId="8_{FE9455B0-5B2A-4DB4-82A5-15E64594C531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C754C31D-4731-45D5-97C2-7D484B1140D9}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{96CFF409-1B85-4529-8B3F-3BC658A689A0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{96CFF409-1B85-4529-8B3F-3BC658A689A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="74">
   <si>
     <t>Month</t>
   </si>
@@ -150,13 +152,247 @@
   </si>
   <si>
     <t>User Testing</t>
+  </si>
+  <si>
+    <r>
+      <t>13</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Nov</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Nov</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>27</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Nov</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Dec</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>11</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Dec</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>18</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Dec</t>
+    </r>
+  </si>
+  <si>
+    <t>Create the survey</t>
+  </si>
+  <si>
+    <t>Send out survey to collect response</t>
+  </si>
+  <si>
+    <t>Complete wireframing</t>
+  </si>
+  <si>
+    <t>Complete prototyping</t>
+  </si>
+  <si>
+    <t>Test prototypes</t>
+  </si>
+  <si>
+    <t>Complete diagrams</t>
+  </si>
+  <si>
+    <t>Work on the login, register and home pages should be implemented</t>
+  </si>
+  <si>
+    <t>31st December</t>
+  </si>
+  <si>
+    <t>Start working on the templates for the cultural learning (scenarios)</t>
+  </si>
+  <si>
+    <t>28th January</t>
+  </si>
+  <si>
+    <t>Set up the backend</t>
+  </si>
+  <si>
+    <t>Set up postgresSQL and connect to web application. Create the database and tables</t>
+  </si>
+  <si>
+    <t>1st February</t>
+  </si>
+  <si>
+    <t>Create discussion forum pages</t>
+  </si>
+  <si>
+    <t>Create the 3 pages for the discussion forum and sync to the backend</t>
+  </si>
+  <si>
+    <t>12th February</t>
+  </si>
+  <si>
+    <t>25th February</t>
+  </si>
+  <si>
+    <t>3rd March</t>
+  </si>
+  <si>
+    <t>10th March</t>
+  </si>
+  <si>
+    <t>Link the login and registration pages to the backend</t>
+  </si>
+  <si>
+    <t>Details from the form inputs should successfully be submitted to the database</t>
+  </si>
+  <si>
+    <t>22nd March</t>
+  </si>
+  <si>
+    <t>Conduct final set of user testing</t>
+  </si>
+  <si>
+    <t>5th April</t>
+  </si>
+  <si>
+    <t>19th April</t>
+  </si>
+  <si>
+    <t>Participants should've been contacted and consent should have been given for testing to happen. A time should have been arranged. Evaluations would be conducted with users using SUS, usability heuristic and TAM</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>February</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,16 +424,65 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFC000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA6A6A6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -220,11 +505,102 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -245,9 +621,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -259,6 +632,90 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -275,6 +732,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -576,17 +1037,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45F5631A-038F-4158-A54D-FDED9211567E}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="35.7109375" style="10" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="35.7109375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -607,134 +1068,134 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="57" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="9" t="s">
+      <c r="A3" s="12"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="57" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="9" t="s">
+      <c r="A4" s="12"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="9" t="s">
+      <c r="A5" s="12"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="10" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="71.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7" t="s">
+      <c r="A6" s="12"/>
+      <c r="B6" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" ht="57" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="9" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="57" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7" t="s">
+      <c r="A8" s="12"/>
+      <c r="B8" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="10" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="57" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="9" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="10" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="8" t="s">
+      <c r="A10" s="39"/>
+      <c r="B10" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="10" t="s">
         <v>33</v>
       </c>
     </row>
@@ -750,4 +1211,329 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96335D66-2677-463F-902C-D22AC44046B8}">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="34" customWidth="1"/>
+    <col min="2" max="2" width="21" style="34" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" style="34" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" style="34" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" style="34" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="111" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="37" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="37" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="37" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+      <c r="B6" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="37" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="37" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12"/>
+      <c r="B8" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="37" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="37" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="142.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="H10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="37" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B2:B5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CF9569B-3EDE-4D6C-A9F8-96CCBFB3FBA1}">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="7" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14"/>
+      <c r="B1" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="17"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+    </row>
+    <row r="3" spans="1:7" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+    </row>
+    <row r="4" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+    </row>
+    <row r="5" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="18"/>
+    </row>
+    <row r="6" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="17"/>
+    </row>
+    <row r="7" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="26"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="32"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="25"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="33"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="35"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>